<commit_message>
Backup QR Scanner data - 2025-10-02T16:26:33.634Z - Cache Bust: 1759422393634
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_Chest_scanner1759316690254_09451dc814cb943b9eea94aa120bd70744ae86a228bc509ddc9ce4cdcb7460d0.xlsx
+++ b/log_history/Y4_B2526_Chest_scanner1759316690254_09451dc814cb943b9eea94aa120bd70744ae86a228bc509ddc9ce4cdcb7460d0.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -424,16 +424,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>221751</v>
+        <v>221672</v>
       </c>
       <c r="B2" t="str">
         <v>Chest</v>
       </c>
       <c r="C2" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D2" t="str">
-        <v>14:05:19</v>
+        <v>19:17:37</v>
       </c>
       <c r="E2" t="str">
         <v>Manual</v>
@@ -444,16 +444,16 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>221655</v>
+        <v>221713</v>
       </c>
       <c r="B3" t="str">
         <v>Chest</v>
       </c>
       <c r="C3" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D3" t="str">
-        <v>14:05:34</v>
+        <v>19:17:44</v>
       </c>
       <c r="E3" t="str">
         <v>Manual</v>
@@ -464,16 +464,16 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>221605</v>
+        <v>221582</v>
       </c>
       <c r="B4" t="str">
         <v>Chest</v>
       </c>
       <c r="C4" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D4" t="str">
-        <v>14:06:02</v>
+        <v>19:17:56</v>
       </c>
       <c r="E4" t="str">
         <v>Manual</v>
@@ -484,16 +484,16 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>221722</v>
+        <v>221535</v>
       </c>
       <c r="B5" t="str">
         <v>Chest</v>
       </c>
       <c r="C5" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D5" t="str">
-        <v>14:06:14</v>
+        <v>19:18:05</v>
       </c>
       <c r="E5" t="str">
         <v>Manual</v>
@@ -504,16 +504,16 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>221641</v>
+        <v>221676</v>
       </c>
       <c r="B6" t="str">
         <v>Chest</v>
       </c>
       <c r="C6" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D6" t="str">
-        <v>14:06:28</v>
+        <v>19:18:12</v>
       </c>
       <c r="E6" t="str">
         <v>Manual</v>
@@ -524,16 +524,16 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>221676</v>
+        <v>221722</v>
       </c>
       <c r="B7" t="str">
         <v>Chest</v>
       </c>
       <c r="C7" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D7" t="str">
-        <v>14:06:48</v>
+        <v>19:18:20</v>
       </c>
       <c r="E7" t="str">
         <v>Manual</v>
@@ -544,16 +544,16 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>221535</v>
+        <v>221712</v>
       </c>
       <c r="B8" t="str">
         <v>Chest</v>
       </c>
       <c r="C8" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D8" t="str">
-        <v>14:07:02</v>
+        <v>19:18:49</v>
       </c>
       <c r="E8" t="str">
         <v>Manual</v>
@@ -564,16 +564,16 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>221712</v>
+        <v>221641</v>
       </c>
       <c r="B9" t="str">
         <v>Chest</v>
       </c>
       <c r="C9" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D9" t="str">
-        <v>14:07:13</v>
+        <v>19:19:01</v>
       </c>
       <c r="E9" t="str">
         <v>Manual</v>
@@ -584,16 +584,16 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>221596</v>
+        <v>221655</v>
       </c>
       <c r="B10" t="str">
         <v>Chest</v>
       </c>
       <c r="C10" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D10" t="str">
-        <v>14:07:37</v>
+        <v>19:19:10</v>
       </c>
       <c r="E10" t="str">
         <v>Manual</v>
@@ -604,16 +604,16 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>221608</v>
+        <v>221605</v>
       </c>
       <c r="B11" t="str">
         <v>Chest</v>
       </c>
       <c r="C11" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D11" t="str">
-        <v>14:07:57</v>
+        <v>19:19:21</v>
       </c>
       <c r="E11" t="str">
         <v>Manual</v>
@@ -624,16 +624,16 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>221700</v>
+        <v>221592</v>
       </c>
       <c r="B12" t="str">
         <v>Chest</v>
       </c>
       <c r="C12" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D12" t="str">
-        <v>14:08:04</v>
+        <v>19:19:29</v>
       </c>
       <c r="E12" t="str">
         <v>Manual</v>
@@ -644,16 +644,16 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>221552</v>
+        <v>221658</v>
       </c>
       <c r="B13" t="str">
         <v>Chest</v>
       </c>
       <c r="C13" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D13" t="str">
-        <v>14:09:01</v>
+        <v>19:19:40</v>
       </c>
       <c r="E13" t="str">
         <v>Manual</v>
@@ -664,16 +664,16 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>221542</v>
+        <v>221552</v>
       </c>
       <c r="B14" t="str">
         <v>Chest</v>
       </c>
       <c r="C14" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D14" t="str">
-        <v>14:09:48</v>
+        <v>19:19:54</v>
       </c>
       <c r="E14" t="str">
         <v>Manual</v>
@@ -684,16 +684,16 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>221719</v>
+        <v>221752</v>
       </c>
       <c r="B15" t="str">
         <v>Chest</v>
       </c>
       <c r="C15" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D15" t="str">
-        <v>14:10:57</v>
+        <v>19:20:10</v>
       </c>
       <c r="E15" t="str">
         <v>Manual</v>
@@ -704,16 +704,16 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>221683</v>
+        <v>221751</v>
       </c>
       <c r="B16" t="str">
         <v>Chest</v>
       </c>
       <c r="C16" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D16" t="str">
-        <v>14:11:12</v>
+        <v>19:20:20</v>
       </c>
       <c r="E16" t="str">
         <v>Manual</v>
@@ -724,16 +724,16 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>221594</v>
+        <v>221706</v>
       </c>
       <c r="B17" t="str">
         <v>Chest</v>
       </c>
       <c r="C17" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D17" t="str">
-        <v>14:11:30</v>
+        <v>19:20:30</v>
       </c>
       <c r="E17" t="str">
         <v>Manual</v>
@@ -744,16 +744,16 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>221697</v>
+        <v>221568</v>
       </c>
       <c r="B18" t="str">
         <v>Chest</v>
       </c>
       <c r="C18" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D18" t="str">
-        <v>14:11:44</v>
+        <v>19:20:40</v>
       </c>
       <c r="E18" t="str">
         <v>Manual</v>
@@ -764,16 +764,16 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>221595</v>
+        <v>221719</v>
       </c>
       <c r="B19" t="str">
         <v>Chest</v>
       </c>
       <c r="C19" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D19" t="str">
-        <v>14:12:04</v>
+        <v>19:21:08</v>
       </c>
       <c r="E19" t="str">
         <v>Manual</v>
@@ -784,16 +784,16 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>221713</v>
+        <v>221657</v>
       </c>
       <c r="B20" t="str">
         <v>Chest</v>
       </c>
       <c r="C20" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D20" t="str">
-        <v>14:12:57</v>
+        <v>19:21:23</v>
       </c>
       <c r="E20" t="str">
         <v>Manual</v>
@@ -804,16 +804,16 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>221533</v>
+        <v>221596</v>
       </c>
       <c r="B21" t="str">
         <v>Chest</v>
       </c>
       <c r="C21" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D21" t="str">
-        <v>14:13:14</v>
+        <v>19:21:36</v>
       </c>
       <c r="E21" t="str">
         <v>Manual</v>
@@ -824,16 +824,16 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>221633</v>
+        <v>221621</v>
       </c>
       <c r="B22" t="str">
         <v>Chest</v>
       </c>
       <c r="C22" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D22" t="str">
-        <v>14:13:29</v>
+        <v>19:21:50</v>
       </c>
       <c r="E22" t="str">
         <v>Manual</v>
@@ -844,16 +844,16 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>221672</v>
+        <v>221538</v>
       </c>
       <c r="B23" t="str">
         <v>Chest</v>
       </c>
       <c r="C23" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D23" t="str">
-        <v>14:13:50</v>
+        <v>19:22:03</v>
       </c>
       <c r="E23" t="str">
         <v>Manual</v>
@@ -864,16 +864,16 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>221702</v>
+        <v>221595</v>
       </c>
       <c r="B24" t="str">
         <v>Chest</v>
       </c>
       <c r="C24" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D24" t="str">
-        <v>14:14:04</v>
+        <v>19:22:11</v>
       </c>
       <c r="E24" t="str">
         <v>Manual</v>
@@ -884,16 +884,16 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>221650</v>
+        <v>221642</v>
       </c>
       <c r="B25" t="str">
         <v>Chest</v>
       </c>
       <c r="C25" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D25" t="str">
-        <v>14:14:17</v>
+        <v>19:22:18</v>
       </c>
       <c r="E25" t="str">
         <v>Manual</v>
@@ -904,16 +904,16 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>221581</v>
+        <v>221556</v>
       </c>
       <c r="B26" t="str">
         <v>Chest</v>
       </c>
       <c r="C26" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D26" t="str">
-        <v>14:15:54</v>
+        <v>19:22:44</v>
       </c>
       <c r="E26" t="str">
         <v>Manual</v>
@@ -924,16 +924,16 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>221583</v>
+        <v>221624</v>
       </c>
       <c r="B27" t="str">
         <v>Chest</v>
       </c>
       <c r="C27" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D27" t="str">
-        <v>14:16:08</v>
+        <v>19:22:51</v>
       </c>
       <c r="E27" t="str">
         <v>Manual</v>
@@ -944,16 +944,16 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>221624</v>
+        <v>221745</v>
       </c>
       <c r="B28" t="str">
         <v>Chest</v>
       </c>
       <c r="C28" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D28" t="str">
-        <v>14:16:29</v>
+        <v>19:23:14</v>
       </c>
       <c r="E28" t="str">
         <v>Manual</v>
@@ -964,16 +964,16 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>221688</v>
+        <v>221594</v>
       </c>
       <c r="B29" t="str">
         <v>Chest</v>
       </c>
       <c r="C29" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D29" t="str">
-        <v>14:16:40</v>
+        <v>19:23:23</v>
       </c>
       <c r="E29" t="str">
         <v>Manual</v>
@@ -984,16 +984,16 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>221686</v>
+        <v>221547</v>
       </c>
       <c r="B30" t="str">
         <v>Chest</v>
       </c>
       <c r="C30" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D30" t="str">
-        <v>14:17:05</v>
+        <v>19:23:30</v>
       </c>
       <c r="E30" t="str">
         <v>Manual</v>
@@ -1004,16 +1004,16 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>221716</v>
+        <v>221533</v>
       </c>
       <c r="B31" t="str">
         <v>Chest</v>
       </c>
       <c r="C31" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D31" t="str">
-        <v>14:17:31</v>
+        <v>19:23:41</v>
       </c>
       <c r="E31" t="str">
         <v>Manual</v>
@@ -1024,16 +1024,16 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>221568</v>
+        <v>221674</v>
       </c>
       <c r="B32" t="str">
         <v>Chest</v>
       </c>
       <c r="C32" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D32" t="str">
-        <v>14:17:46</v>
+        <v>19:23:51</v>
       </c>
       <c r="E32" t="str">
         <v>Manual</v>
@@ -1044,16 +1044,16 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>221652</v>
+        <v>221697</v>
       </c>
       <c r="B33" t="str">
         <v>Chest</v>
       </c>
       <c r="C33" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D33" t="str">
-        <v>14:18:03</v>
+        <v>19:24:00</v>
       </c>
       <c r="E33" t="str">
         <v>Manual</v>
@@ -1064,16 +1064,16 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>221701</v>
+        <v>221683</v>
       </c>
       <c r="B34" t="str">
         <v>Chest</v>
       </c>
       <c r="C34" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D34" t="str">
-        <v>14:18:15</v>
+        <v>19:24:08</v>
       </c>
       <c r="E34" t="str">
         <v>Manual</v>
@@ -1084,16 +1084,16 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>221621</v>
+        <v>221694</v>
       </c>
       <c r="B35" t="str">
         <v>Chest</v>
       </c>
       <c r="C35" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D35" t="str">
-        <v>14:18:30</v>
+        <v>19:24:15</v>
       </c>
       <c r="E35" t="str">
         <v>Manual</v>
@@ -1104,16 +1104,16 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>221615</v>
+        <v>221709</v>
       </c>
       <c r="B36" t="str">
         <v>Chest</v>
       </c>
       <c r="C36" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D36" t="str">
-        <v>14:19:12</v>
+        <v>19:24:28</v>
       </c>
       <c r="E36" t="str">
         <v>Manual</v>
@@ -1124,16 +1124,16 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>221592</v>
+        <v>221707</v>
       </c>
       <c r="B37" t="str">
         <v>Chest</v>
       </c>
       <c r="C37" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D37" t="str">
-        <v>14:19:33</v>
+        <v>19:24:36</v>
       </c>
       <c r="E37" t="str">
         <v>Manual</v>
@@ -1144,16 +1144,16 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>221752</v>
+        <v>221689</v>
       </c>
       <c r="B38" t="str">
         <v>Chest</v>
       </c>
       <c r="C38" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D38" t="str">
-        <v>14:20:04</v>
+        <v>19:24:43</v>
       </c>
       <c r="E38" t="str">
         <v>Manual</v>
@@ -1164,27 +1164,207 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>221740</v>
+        <v>221716</v>
       </c>
       <c r="B39" t="str">
         <v>Chest</v>
       </c>
       <c r="C39" t="str">
-        <v>01/10/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="D39" t="str">
-        <v>14:20:17</v>
+        <v>19:24:49</v>
       </c>
       <c r="E39" t="str">
         <v>Manual</v>
       </c>
       <c r="F39" t="str">
+        <v>ahmedali78112@gmail.com</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>221686</v>
+      </c>
+      <c r="B40" t="str">
+        <v>Chest</v>
+      </c>
+      <c r="C40" t="str">
+        <v>02/10/2025</v>
+      </c>
+      <c r="D40" t="str">
+        <v>19:25:05</v>
+      </c>
+      <c r="E40" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F40" t="str">
+        <v>ahmedali78112@gmail.com</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>221711</v>
+      </c>
+      <c r="B41" t="str">
+        <v>Chest</v>
+      </c>
+      <c r="C41" t="str">
+        <v>02/10/2025</v>
+      </c>
+      <c r="D41" t="str">
+        <v>19:25:12</v>
+      </c>
+      <c r="E41" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F41" t="str">
+        <v>ahmedali78112@gmail.com</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>221673</v>
+      </c>
+      <c r="B42" t="str">
+        <v>Chest</v>
+      </c>
+      <c r="C42" t="str">
+        <v>02/10/2025</v>
+      </c>
+      <c r="D42" t="str">
+        <v>19:25:19</v>
+      </c>
+      <c r="E42" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F42" t="str">
+        <v>ahmedali78112@gmail.com</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>221616</v>
+      </c>
+      <c r="B43" t="str">
+        <v>Chest</v>
+      </c>
+      <c r="C43" t="str">
+        <v>02/10/2025</v>
+      </c>
+      <c r="D43" t="str">
+        <v>19:25:40</v>
+      </c>
+      <c r="E43" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F43" t="str">
+        <v>ahmedali78112@gmail.com</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>221542</v>
+      </c>
+      <c r="B44" t="str">
+        <v>Chest</v>
+      </c>
+      <c r="C44" t="str">
+        <v>02/10/2025</v>
+      </c>
+      <c r="D44" t="str">
+        <v>19:25:48</v>
+      </c>
+      <c r="E44" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F44" t="str">
+        <v>ahmedali78112@gmail.com</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>221585</v>
+      </c>
+      <c r="B45" t="str">
+        <v>Chest</v>
+      </c>
+      <c r="C45" t="str">
+        <v>02/10/2025</v>
+      </c>
+      <c r="D45" t="str">
+        <v>19:25:57</v>
+      </c>
+      <c r="E45" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F45" t="str">
+        <v>ahmedali78112@gmail.com</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>221603</v>
+      </c>
+      <c r="B46" t="str">
+        <v>Chest</v>
+      </c>
+      <c r="C46" t="str">
+        <v>02/10/2025</v>
+      </c>
+      <c r="D46" t="str">
+        <v>19:26:05</v>
+      </c>
+      <c r="E46" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F46" t="str">
+        <v>ahmedali78112@gmail.com</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>221677</v>
+      </c>
+      <c r="B47" t="str">
+        <v>Chest</v>
+      </c>
+      <c r="C47" t="str">
+        <v>02/10/2025</v>
+      </c>
+      <c r="D47" t="str">
+        <v>19:26:11</v>
+      </c>
+      <c r="E47" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F47" t="str">
+        <v>ahmedali78112@gmail.com</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>180915</v>
+      </c>
+      <c r="B48" t="str">
+        <v>Chest</v>
+      </c>
+      <c r="C48" t="str">
+        <v>02/10/2025</v>
+      </c>
+      <c r="D48" t="str">
+        <v>19:26:18</v>
+      </c>
+      <c r="E48" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F48" t="str">
         <v>ahmedali78112@gmail.com</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F39"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F48"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Backup QR Scanner data - 2025-10-05T03:13:16.371Z - Cache Bust: 1759633996371
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_Chest_scanner1759316690254_09451dc814cb943b9eea94aa120bd70744ae86a228bc509ddc9ce4cdcb7460d0.xlsx
+++ b/log_history/Y4_B2526_Chest_scanner1759316690254_09451dc814cb943b9eea94aa120bd70744ae86a228bc509ddc9ce4cdcb7460d0.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Scanner" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -424,16 +424,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>221672</v>
+        <v>221751</v>
       </c>
       <c r="B2" t="str">
         <v>Chest</v>
       </c>
       <c r="C2" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D2" t="str">
-        <v>19:17:37</v>
+        <v>14:05:19</v>
       </c>
       <c r="E2" t="str">
         <v>Manual</v>
@@ -444,16 +444,16 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>221713</v>
+        <v>221655</v>
       </c>
       <c r="B3" t="str">
         <v>Chest</v>
       </c>
       <c r="C3" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D3" t="str">
-        <v>19:17:44</v>
+        <v>14:05:34</v>
       </c>
       <c r="E3" t="str">
         <v>Manual</v>
@@ -464,16 +464,16 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>221582</v>
+        <v>221605</v>
       </c>
       <c r="B4" t="str">
         <v>Chest</v>
       </c>
       <c r="C4" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D4" t="str">
-        <v>19:17:56</v>
+        <v>14:06:02</v>
       </c>
       <c r="E4" t="str">
         <v>Manual</v>
@@ -484,16 +484,16 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>221535</v>
+        <v>221722</v>
       </c>
       <c r="B5" t="str">
         <v>Chest</v>
       </c>
       <c r="C5" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D5" t="str">
-        <v>19:18:05</v>
+        <v>14:06:14</v>
       </c>
       <c r="E5" t="str">
         <v>Manual</v>
@@ -504,16 +504,16 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>221676</v>
+        <v>221641</v>
       </c>
       <c r="B6" t="str">
         <v>Chest</v>
       </c>
       <c r="C6" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D6" t="str">
-        <v>19:18:12</v>
+        <v>14:06:28</v>
       </c>
       <c r="E6" t="str">
         <v>Manual</v>
@@ -524,16 +524,16 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>221722</v>
+        <v>221676</v>
       </c>
       <c r="B7" t="str">
         <v>Chest</v>
       </c>
       <c r="C7" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D7" t="str">
-        <v>19:18:20</v>
+        <v>14:06:48</v>
       </c>
       <c r="E7" t="str">
         <v>Manual</v>
@@ -544,16 +544,16 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>221712</v>
+        <v>221535</v>
       </c>
       <c r="B8" t="str">
         <v>Chest</v>
       </c>
       <c r="C8" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D8" t="str">
-        <v>19:18:49</v>
+        <v>14:07:02</v>
       </c>
       <c r="E8" t="str">
         <v>Manual</v>
@@ -564,16 +564,16 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>221641</v>
+        <v>221712</v>
       </c>
       <c r="B9" t="str">
         <v>Chest</v>
       </c>
       <c r="C9" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D9" t="str">
-        <v>19:19:01</v>
+        <v>14:07:13</v>
       </c>
       <c r="E9" t="str">
         <v>Manual</v>
@@ -584,16 +584,16 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>221655</v>
+        <v>221596</v>
       </c>
       <c r="B10" t="str">
         <v>Chest</v>
       </c>
       <c r="C10" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D10" t="str">
-        <v>19:19:10</v>
+        <v>14:07:37</v>
       </c>
       <c r="E10" t="str">
         <v>Manual</v>
@@ -604,16 +604,16 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>221605</v>
+        <v>221608</v>
       </c>
       <c r="B11" t="str">
         <v>Chest</v>
       </c>
       <c r="C11" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D11" t="str">
-        <v>19:19:21</v>
+        <v>14:07:57</v>
       </c>
       <c r="E11" t="str">
         <v>Manual</v>
@@ -624,16 +624,16 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>221592</v>
+        <v>221700</v>
       </c>
       <c r="B12" t="str">
         <v>Chest</v>
       </c>
       <c r="C12" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D12" t="str">
-        <v>19:19:29</v>
+        <v>14:08:04</v>
       </c>
       <c r="E12" t="str">
         <v>Manual</v>
@@ -644,16 +644,16 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>221658</v>
+        <v>221552</v>
       </c>
       <c r="B13" t="str">
         <v>Chest</v>
       </c>
       <c r="C13" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D13" t="str">
-        <v>19:19:40</v>
+        <v>14:09:01</v>
       </c>
       <c r="E13" t="str">
         <v>Manual</v>
@@ -664,16 +664,16 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>221552</v>
+        <v>221542</v>
       </c>
       <c r="B14" t="str">
         <v>Chest</v>
       </c>
       <c r="C14" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D14" t="str">
-        <v>19:19:54</v>
+        <v>14:09:48</v>
       </c>
       <c r="E14" t="str">
         <v>Manual</v>
@@ -684,16 +684,16 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>221752</v>
+        <v>221719</v>
       </c>
       <c r="B15" t="str">
         <v>Chest</v>
       </c>
       <c r="C15" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D15" t="str">
-        <v>19:20:10</v>
+        <v>14:10:57</v>
       </c>
       <c r="E15" t="str">
         <v>Manual</v>
@@ -704,16 +704,16 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>221751</v>
+        <v>221683</v>
       </c>
       <c r="B16" t="str">
         <v>Chest</v>
       </c>
       <c r="C16" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D16" t="str">
-        <v>19:20:20</v>
+        <v>14:11:12</v>
       </c>
       <c r="E16" t="str">
         <v>Manual</v>
@@ -724,16 +724,16 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>221706</v>
+        <v>221594</v>
       </c>
       <c r="B17" t="str">
         <v>Chest</v>
       </c>
       <c r="C17" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D17" t="str">
-        <v>19:20:30</v>
+        <v>14:11:30</v>
       </c>
       <c r="E17" t="str">
         <v>Manual</v>
@@ -744,16 +744,16 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>221568</v>
+        <v>221697</v>
       </c>
       <c r="B18" t="str">
         <v>Chest</v>
       </c>
       <c r="C18" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D18" t="str">
-        <v>19:20:40</v>
+        <v>14:11:44</v>
       </c>
       <c r="E18" t="str">
         <v>Manual</v>
@@ -764,16 +764,16 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>221719</v>
+        <v>221595</v>
       </c>
       <c r="B19" t="str">
         <v>Chest</v>
       </c>
       <c r="C19" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D19" t="str">
-        <v>19:21:08</v>
+        <v>14:12:04</v>
       </c>
       <c r="E19" t="str">
         <v>Manual</v>
@@ -784,16 +784,16 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>221657</v>
+        <v>221713</v>
       </c>
       <c r="B20" t="str">
         <v>Chest</v>
       </c>
       <c r="C20" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D20" t="str">
-        <v>19:21:23</v>
+        <v>14:12:57</v>
       </c>
       <c r="E20" t="str">
         <v>Manual</v>
@@ -804,16 +804,16 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>221596</v>
+        <v>221533</v>
       </c>
       <c r="B21" t="str">
         <v>Chest</v>
       </c>
       <c r="C21" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D21" t="str">
-        <v>19:21:36</v>
+        <v>14:13:14</v>
       </c>
       <c r="E21" t="str">
         <v>Manual</v>
@@ -824,16 +824,16 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>221621</v>
+        <v>221633</v>
       </c>
       <c r="B22" t="str">
         <v>Chest</v>
       </c>
       <c r="C22" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D22" t="str">
-        <v>19:21:50</v>
+        <v>14:13:29</v>
       </c>
       <c r="E22" t="str">
         <v>Manual</v>
@@ -844,16 +844,16 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>221538</v>
+        <v>221672</v>
       </c>
       <c r="B23" t="str">
         <v>Chest</v>
       </c>
       <c r="C23" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D23" t="str">
-        <v>19:22:03</v>
+        <v>14:13:50</v>
       </c>
       <c r="E23" t="str">
         <v>Manual</v>
@@ -864,16 +864,16 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>221595</v>
+        <v>221702</v>
       </c>
       <c r="B24" t="str">
         <v>Chest</v>
       </c>
       <c r="C24" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D24" t="str">
-        <v>19:22:11</v>
+        <v>14:14:04</v>
       </c>
       <c r="E24" t="str">
         <v>Manual</v>
@@ -884,16 +884,16 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>221642</v>
+        <v>221650</v>
       </c>
       <c r="B25" t="str">
         <v>Chest</v>
       </c>
       <c r="C25" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D25" t="str">
-        <v>19:22:18</v>
+        <v>14:14:17</v>
       </c>
       <c r="E25" t="str">
         <v>Manual</v>
@@ -904,16 +904,16 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>221556</v>
+        <v>221581</v>
       </c>
       <c r="B26" t="str">
         <v>Chest</v>
       </c>
       <c r="C26" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D26" t="str">
-        <v>19:22:44</v>
+        <v>14:15:54</v>
       </c>
       <c r="E26" t="str">
         <v>Manual</v>
@@ -924,16 +924,16 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>221624</v>
+        <v>221583</v>
       </c>
       <c r="B27" t="str">
         <v>Chest</v>
       </c>
       <c r="C27" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D27" t="str">
-        <v>19:22:51</v>
+        <v>14:16:08</v>
       </c>
       <c r="E27" t="str">
         <v>Manual</v>
@@ -944,16 +944,16 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>221745</v>
+        <v>221624</v>
       </c>
       <c r="B28" t="str">
         <v>Chest</v>
       </c>
       <c r="C28" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D28" t="str">
-        <v>19:23:14</v>
+        <v>14:16:29</v>
       </c>
       <c r="E28" t="str">
         <v>Manual</v>
@@ -964,16 +964,16 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>221594</v>
+        <v>221688</v>
       </c>
       <c r="B29" t="str">
         <v>Chest</v>
       </c>
       <c r="C29" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D29" t="str">
-        <v>19:23:23</v>
+        <v>14:16:40</v>
       </c>
       <c r="E29" t="str">
         <v>Manual</v>
@@ -984,16 +984,16 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>221547</v>
+        <v>221686</v>
       </c>
       <c r="B30" t="str">
         <v>Chest</v>
       </c>
       <c r="C30" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D30" t="str">
-        <v>19:23:30</v>
+        <v>14:17:05</v>
       </c>
       <c r="E30" t="str">
         <v>Manual</v>
@@ -1004,16 +1004,16 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>221533</v>
+        <v>221716</v>
       </c>
       <c r="B31" t="str">
         <v>Chest</v>
       </c>
       <c r="C31" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D31" t="str">
-        <v>19:23:41</v>
+        <v>14:17:31</v>
       </c>
       <c r="E31" t="str">
         <v>Manual</v>
@@ -1024,16 +1024,16 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>221674</v>
+        <v>221568</v>
       </c>
       <c r="B32" t="str">
         <v>Chest</v>
       </c>
       <c r="C32" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D32" t="str">
-        <v>19:23:51</v>
+        <v>14:17:46</v>
       </c>
       <c r="E32" t="str">
         <v>Manual</v>
@@ -1044,16 +1044,16 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>221697</v>
+        <v>221652</v>
       </c>
       <c r="B33" t="str">
         <v>Chest</v>
       </c>
       <c r="C33" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D33" t="str">
-        <v>19:24:00</v>
+        <v>14:18:03</v>
       </c>
       <c r="E33" t="str">
         <v>Manual</v>
@@ -1064,16 +1064,16 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>221683</v>
+        <v>221701</v>
       </c>
       <c r="B34" t="str">
         <v>Chest</v>
       </c>
       <c r="C34" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D34" t="str">
-        <v>19:24:08</v>
+        <v>14:18:15</v>
       </c>
       <c r="E34" t="str">
         <v>Manual</v>
@@ -1084,16 +1084,16 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>221694</v>
+        <v>221621</v>
       </c>
       <c r="B35" t="str">
         <v>Chest</v>
       </c>
       <c r="C35" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D35" t="str">
-        <v>19:24:15</v>
+        <v>14:18:30</v>
       </c>
       <c r="E35" t="str">
         <v>Manual</v>
@@ -1104,16 +1104,16 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>221709</v>
+        <v>221615</v>
       </c>
       <c r="B36" t="str">
         <v>Chest</v>
       </c>
       <c r="C36" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D36" t="str">
-        <v>19:24:28</v>
+        <v>14:19:12</v>
       </c>
       <c r="E36" t="str">
         <v>Manual</v>
@@ -1124,16 +1124,16 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>221707</v>
+        <v>221592</v>
       </c>
       <c r="B37" t="str">
         <v>Chest</v>
       </c>
       <c r="C37" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D37" t="str">
-        <v>19:24:36</v>
+        <v>14:19:33</v>
       </c>
       <c r="E37" t="str">
         <v>Manual</v>
@@ -1144,16 +1144,16 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>221689</v>
+        <v>221752</v>
       </c>
       <c r="B38" t="str">
         <v>Chest</v>
       </c>
       <c r="C38" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D38" t="str">
-        <v>19:24:43</v>
+        <v>14:20:04</v>
       </c>
       <c r="E38" t="str">
         <v>Manual</v>
@@ -1164,207 +1164,27 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>221716</v>
+        <v>221740</v>
       </c>
       <c r="B39" t="str">
         <v>Chest</v>
       </c>
       <c r="C39" t="str">
-        <v>02/10/2025</v>
+        <v>01/10/2025</v>
       </c>
       <c r="D39" t="str">
-        <v>19:24:49</v>
+        <v>14:20:17</v>
       </c>
       <c r="E39" t="str">
         <v>Manual</v>
       </c>
       <c r="F39" t="str">
-        <v>ahmedali78112@gmail.com</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="str">
-        <v>221686</v>
-      </c>
-      <c r="B40" t="str">
-        <v>Chest</v>
-      </c>
-      <c r="C40" t="str">
-        <v>02/10/2025</v>
-      </c>
-      <c r="D40" t="str">
-        <v>19:25:05</v>
-      </c>
-      <c r="E40" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F40" t="str">
-        <v>ahmedali78112@gmail.com</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="str">
-        <v>221711</v>
-      </c>
-      <c r="B41" t="str">
-        <v>Chest</v>
-      </c>
-      <c r="C41" t="str">
-        <v>02/10/2025</v>
-      </c>
-      <c r="D41" t="str">
-        <v>19:25:12</v>
-      </c>
-      <c r="E41" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F41" t="str">
-        <v>ahmedali78112@gmail.com</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="str">
-        <v>221673</v>
-      </c>
-      <c r="B42" t="str">
-        <v>Chest</v>
-      </c>
-      <c r="C42" t="str">
-        <v>02/10/2025</v>
-      </c>
-      <c r="D42" t="str">
-        <v>19:25:19</v>
-      </c>
-      <c r="E42" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F42" t="str">
-        <v>ahmedali78112@gmail.com</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="str">
-        <v>221616</v>
-      </c>
-      <c r="B43" t="str">
-        <v>Chest</v>
-      </c>
-      <c r="C43" t="str">
-        <v>02/10/2025</v>
-      </c>
-      <c r="D43" t="str">
-        <v>19:25:40</v>
-      </c>
-      <c r="E43" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F43" t="str">
-        <v>ahmedali78112@gmail.com</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="str">
-        <v>221542</v>
-      </c>
-      <c r="B44" t="str">
-        <v>Chest</v>
-      </c>
-      <c r="C44" t="str">
-        <v>02/10/2025</v>
-      </c>
-      <c r="D44" t="str">
-        <v>19:25:48</v>
-      </c>
-      <c r="E44" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F44" t="str">
-        <v>ahmedali78112@gmail.com</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="str">
-        <v>221585</v>
-      </c>
-      <c r="B45" t="str">
-        <v>Chest</v>
-      </c>
-      <c r="C45" t="str">
-        <v>02/10/2025</v>
-      </c>
-      <c r="D45" t="str">
-        <v>19:25:57</v>
-      </c>
-      <c r="E45" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F45" t="str">
-        <v>ahmedali78112@gmail.com</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="str">
-        <v>221603</v>
-      </c>
-      <c r="B46" t="str">
-        <v>Chest</v>
-      </c>
-      <c r="C46" t="str">
-        <v>02/10/2025</v>
-      </c>
-      <c r="D46" t="str">
-        <v>19:26:05</v>
-      </c>
-      <c r="E46" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F46" t="str">
-        <v>ahmedali78112@gmail.com</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="str">
-        <v>221677</v>
-      </c>
-      <c r="B47" t="str">
-        <v>Chest</v>
-      </c>
-      <c r="C47" t="str">
-        <v>02/10/2025</v>
-      </c>
-      <c r="D47" t="str">
-        <v>19:26:11</v>
-      </c>
-      <c r="E47" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F47" t="str">
-        <v>ahmedali78112@gmail.com</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="str">
-        <v>180915</v>
-      </c>
-      <c r="B48" t="str">
-        <v>Chest</v>
-      </c>
-      <c r="C48" t="str">
-        <v>02/10/2025</v>
-      </c>
-      <c r="D48" t="str">
-        <v>19:26:18</v>
-      </c>
-      <c r="E48" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F48" t="str">
         <v>ahmedali78112@gmail.com</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F48"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F39"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>